<commit_message>
CNA analysis update:     * trying to fit Ndecay and Npeak curves to experimental data;
</commit_message>
<xml_diff>
--- a/CNA/Calibrations/Detectors_E-Calib.xlsx
+++ b/CNA/Calibrations/Detectors_E-Calib.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28318"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\OneDrive - Universidade de Lisboa\NUCRIA\TESE\Activations\116Sn(p,g)117Sb_Analysis\CNA\Calibrations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_6D59A76F99683EB83AAFF0829EC629416EC23B67" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="7040" tabRatio="749" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="7035" tabRatio="749" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="152Eu" sheetId="1" r:id="rId1"/>
@@ -20,8 +19,9 @@
     <sheet name="Background" sheetId="5" r:id="rId5"/>
     <sheet name="Energy Calibration" sheetId="6" r:id="rId6"/>
     <sheet name="Resolution" sheetId="7" r:id="rId7"/>
+    <sheet name="117Sb Decay" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="191028" iterateDelta="1E-4"/>
+  <calcPr calcId="152511" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="84">
   <si>
     <t>Energy (keV)</t>
   </si>
@@ -289,20 +289,29 @@
   <si>
     <t>Need to use these values to perform energy calibration</t>
   </si>
+  <si>
+    <t>eta</t>
+  </si>
+  <si>
+    <t>Resolution</t>
+  </si>
+  <si>
+    <t>Relative intensity (%)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="6">
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="166" formatCode="0.0000"/>
-    <numFmt numFmtId="167" formatCode="_-* #,##0.0000\ _€_-;\-* #,##0.0000\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
-    <numFmt numFmtId="168" formatCode="0.00000"/>
-    <numFmt numFmtId="169" formatCode="_-* #,##0.00000\ _€_-;\-* #,##0.00000\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0.0000\ _€_-;\-* #,##0.0000\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="0.00000"/>
+    <numFmt numFmtId="168" formatCode="_-* #,##0.00000\ _€_-;\-* #,##0.00000\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -782,9 +791,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="294">
+  <cellXfs count="300">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -904,7 +913,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -949,13 +958,13 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -967,16 +976,16 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -985,7 +994,7 @@
     <xf numFmtId="2" fontId="8" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1018,52 +1027,52 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1072,13 +1081,13 @@
     <xf numFmtId="2" fontId="8" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1093,7 +1102,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="13" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="13" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1108,7 +1117,7 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="13" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -1413,7 +1422,7 @@
     <xf numFmtId="1" fontId="0" fillId="14" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="13" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="13" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1428,7 +1437,7 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="13" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="13" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1504,16 +1513,16 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1540,28 +1549,28 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="8" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1576,7 +1585,7 @@
     <xf numFmtId="2" fontId="8" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1591,19 +1600,19 @@
     <xf numFmtId="2" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="13" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="13" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="13" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="13" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1621,10 +1630,28 @@
     <xf numFmtId="0" fontId="3" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Vírgula" xfId="1" builtinId="3"/>
   </cellStyles>
   <dxfs count="26">
     <dxf>
@@ -1642,7 +1669,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="_-* #,##0.0000\ _€_-;\-* #,##0.0000\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
+      <numFmt numFmtId="166" formatCode="_-* #,##0.0000\ _€_-;\-* #,##0.0000\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1682,11 +1709,14 @@
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode="0.0000"/>
+      <numFmt numFmtId="165" formatCode="0.0000"/>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1698,9 +1728,6 @@
           <color indexed="64"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1892,9 +1919,9 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="pt-PT"/>
   <c:roundedCorners val="0"/>
   <c:style val="2"/>
   <c:chart>
@@ -1991,7 +2018,7 @@
                     <a:latin typeface="Calibri"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="pt-PT"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="r"/>
@@ -2003,7 +2030,7 @@
             <c:showBubbleSize val="1"/>
             <c:separator>; </c:separator>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -2035,6 +2062,10 @@
                         </a:solidFill>
                       </a:rPr>
                       <a:t>y = 0,0310589x - 0,0041372</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t/>
                     </a:r>
                     <a:br>
                       <a:rPr lang="en-US" baseline="0"/>
@@ -2163,7 +2194,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-F97F-464F-8EF8-0A58DE08EF11}"/>
             </c:ext>
@@ -2177,11 +2208,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="627023904"/>
-        <c:axId val="627027712"/>
+        <c:axId val="-1817143696"/>
+        <c:axId val="-1817146960"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="627023904"/>
+        <c:axId val="-1817143696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2255,15 +2286,15 @@
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="627027712"/>
+        <c:crossAx val="-1817146960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="627027712"/>
+        <c:axId val="-1817146960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2345,10 +2376,10 @@
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="627023904"/>
+        <c:crossAx val="-1817143696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2383,9 +2414,9 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="pt-PT"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2459,7 +2490,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-PT"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2522,7 +2553,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="pt-PT"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="r"/>
@@ -2534,7 +2565,7 @@
             <c:showBubbleSize val="1"/>
             <c:separator>; </c:separator>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -2584,6 +2615,10 @@
                       </a:rPr>
                       <a:t>y = 0,32252559x - 0,45562629</a:t>
                     </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t/>
+                    </a:r>
                     <a:br>
                       <a:rPr lang="en-US" baseline="0"/>
                     </a:br>
@@ -2621,7 +2656,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="pt-PT"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -2747,7 +2782,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-B850-4637-9D13-11CBBB845B9D}"/>
             </c:ext>
@@ -2761,11 +2796,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="627022816"/>
-        <c:axId val="627030432"/>
+        <c:axId val="-1817143152"/>
+        <c:axId val="-1817151856"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="627022816"/>
+        <c:axId val="-1817143152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2833,7 +2868,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="pt-PT"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2866,15 +2901,15 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="627030432"/>
+        <c:crossAx val="-1817151856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="627030432"/>
+        <c:axId val="-1817151856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2950,7 +2985,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="pt-PT"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2983,10 +3018,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="627022816"/>
+        <c:crossAx val="-1817143152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3022,7 +3057,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="pt-PT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3034,9 +3069,9 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="pt-PT"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3110,7 +3145,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-PT"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3170,7 +3205,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="pt-PT"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="r"/>
@@ -3182,7 +3217,7 @@
             <c:showBubbleSize val="1"/>
             <c:separator>; </c:separator>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -3249,6 +3284,10 @@
                       </a:rPr>
                       <a:t> - 0,000427x + 0,000702</a:t>
                     </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t/>
+                    </a:r>
                     <a:br>
                       <a:rPr lang="en-US" baseline="0"/>
                     </a:br>
@@ -3286,7 +3325,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="pt-PT"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -3300,7 +3339,7 @@
               <c:numRef>
                 <c:f>Resolution!$O$4:$O$24</c:f>
                 <c:numCache>
-                  <c:formatCode>0.00000</c:formatCode>
+                  <c:formatCode>General</c:formatCode>
                   <c:ptCount val="21"/>
                   <c:pt idx="0">
                     <c:v>6.2370484845623259E-5</c:v>
@@ -3372,7 +3411,7 @@
               <c:numRef>
                 <c:f>Resolution!$O$4:$O$24</c:f>
                 <c:numCache>
-                  <c:formatCode>0.00000</c:formatCode>
+                  <c:formatCode>General</c:formatCode>
                   <c:ptCount val="21"/>
                   <c:pt idx="0">
                     <c:v>6.2370484845623259E-5</c:v>
@@ -3619,7 +3658,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-E7EB-4B6A-BF95-C96C206A7788}"/>
             </c:ext>
@@ -3633,11 +3672,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="627028256"/>
-        <c:axId val="627028800"/>
+        <c:axId val="-1817149680"/>
+        <c:axId val="-1817145328"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="627028256"/>
+        <c:axId val="-1817149680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3683,6 +3722,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3705,7 +3745,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="pt-PT"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3738,15 +3778,15 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="627028800"/>
+        <c:crossAx val="-1817145328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="627028800"/>
+        <c:axId val="-1817145328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3792,6 +3832,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3814,7 +3855,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="pt-PT"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3847,10 +3888,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="627028256"/>
+        <c:crossAx val="-1817149680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3886,7 +3927,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="pt-PT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3898,9 +3939,9 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="pt-PT"/>
   <c:roundedCorners val="0"/>
   <c:style val="2"/>
   <c:chart>
@@ -3994,7 +4035,7 @@
                     <a:latin typeface="Calibri"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="pt-PT"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="r"/>
@@ -4006,7 +4047,7 @@
             <c:showBubbleSize val="1"/>
             <c:separator>; </c:separator>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -4045,7 +4086,7 @@
               <c:numRef>
                 <c:f>Resolution!$O$26:$O$40</c:f>
                 <c:numCache>
-                  <c:formatCode>0.00000</c:formatCode>
+                  <c:formatCode>General</c:formatCode>
                   <c:ptCount val="15"/>
                   <c:pt idx="0">
                     <c:v>6.827884200700118E-4</c:v>
@@ -4099,7 +4140,7 @@
               <c:numRef>
                 <c:f>Resolution!$O$26:$O$40</c:f>
                 <c:numCache>
-                  <c:formatCode>0.00000</c:formatCode>
+                  <c:formatCode>General</c:formatCode>
                   <c:ptCount val="15"/>
                   <c:pt idx="0">
                     <c:v>6.827884200700118E-4</c:v>
@@ -4259,7 +4300,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-78D7-41B8-B3B6-C592AA9A404E}"/>
             </c:ext>
@@ -4273,11 +4314,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="627023360"/>
-        <c:axId val="627030976"/>
+        <c:axId val="-1817140432"/>
+        <c:axId val="-1817139888"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="627023360"/>
+        <c:axId val="-1817140432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4319,6 +4360,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4351,15 +4393,15 @@
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="627030976"/>
+        <c:crossAx val="-1817139888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="627030976"/>
+        <c:axId val="-1817139888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4401,6 +4443,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4433,10 +4476,10 @@
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="627023360"/>
+        <c:crossAx val="-1817140432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5428,7 +5471,7 @@
         <xdr:cNvPr id="2" name="Gráfico 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5464,7 +5507,7 @@
         <xdr:cNvPr id="3" name="Gráfico 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5505,7 +5548,7 @@
         <xdr:cNvPr id="4" name="Gráfico 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0600-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5541,7 +5584,7 @@
         <xdr:cNvPr id="5" name="Gráfico 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0600-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5563,8 +5606,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="B2:F203" totalsRowShown="0" headerRowDxfId="25" headerRowBorderDxfId="24">
-  <autoFilter ref="B2:F203" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B2:F203" totalsRowShown="0" headerRowDxfId="25" headerRowBorderDxfId="24">
+  <autoFilter ref="B2:F203">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -5572,19 +5615,19 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Energy (keV)" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="intensity (%)"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="shell"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="HPGe Channel"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="SDD Channel" dataDxfId="22"/>
+    <tableColumn id="1" name="Energy (keV)" dataDxfId="23"/>
+    <tableColumn id="2" name="intensity (%)"/>
+    <tableColumn id="3" name="shell"/>
+    <tableColumn id="4" name="HPGe Channel"/>
+    <tableColumn id="5" name="SDD Channel" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabela2" displayName="Tabela2" ref="B2:I36" totalsRowShown="0" headerRowDxfId="21" tableBorderDxfId="20">
-  <autoFilter ref="B2:I36" xr:uid="{00000000-0009-0000-0100-000002000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="B2:I36" totalsRowShown="0" headerRowDxfId="21" tableBorderDxfId="20">
+  <autoFilter ref="B2:I36">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -5595,22 +5638,22 @@
     <filterColumn colId="7" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Source"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Line"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Parent"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Shell" dataDxfId="19"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Energy (keV)" dataDxfId="18"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="SDD Channel" dataDxfId="17"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="HPGe Channel"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Mean energy (keV)"/>
+    <tableColumn id="1" name="Source"/>
+    <tableColumn id="2" name="Line"/>
+    <tableColumn id="3" name="Parent"/>
+    <tableColumn id="4" name="Shell" dataDxfId="19"/>
+    <tableColumn id="5" name="Energy (keV)" dataDxfId="18"/>
+    <tableColumn id="7" name="SDD Channel" dataDxfId="17"/>
+    <tableColumn id="10" name="HPGe Channel"/>
+    <tableColumn id="11" name="Mean energy (keV)"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Tabela3" displayName="Tabela3" ref="B3:O41" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15" headerRowBorderDxfId="14">
-  <autoFilter ref="B3:O41" xr:uid="{00000000-0009-0000-0100-000003000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabela3" displayName="Tabela3" ref="B3:O41" totalsRowShown="0" headerRowDxfId="16" dataDxfId="14" headerRowBorderDxfId="15">
+  <autoFilter ref="B3:O41">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -5627,22 +5670,22 @@
     <filterColumn colId="13" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Peak nr." dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name=" Energy (keV) " dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Energy (MeV)" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name=" ROId " dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name=" ROIu " dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Centroid " dataDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name=" Sigma " dataDxfId="7"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="dSigma" dataDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name=" FWHM " dataDxfId="5"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="FWHM (MeV)" dataDxfId="4"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="dFWHM (MeV)" dataDxfId="3"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0200-00000D000000}" name="1/sqrt(E') (MeV)^-0.5" dataDxfId="2"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0200-00000E000000}" name="R = FWHM/E" dataDxfId="1">
+    <tableColumn id="1" name="Peak nr." dataDxfId="13"/>
+    <tableColumn id="2" name=" Energy (keV) " dataDxfId="12"/>
+    <tableColumn id="3" name="Energy (MeV)" dataDxfId="11"/>
+    <tableColumn id="4" name=" ROId " dataDxfId="10"/>
+    <tableColumn id="5" name=" ROIu " dataDxfId="9"/>
+    <tableColumn id="6" name="Centroid " dataDxfId="8"/>
+    <tableColumn id="7" name=" Sigma " dataDxfId="7"/>
+    <tableColumn id="8" name="dSigma" dataDxfId="6"/>
+    <tableColumn id="9" name=" FWHM " dataDxfId="5"/>
+    <tableColumn id="10" name="FWHM (MeV)" dataDxfId="4"/>
+    <tableColumn id="11" name="dFWHM (MeV)" dataDxfId="3"/>
+    <tableColumn id="13" name="1/sqrt(E') (MeV)^-0.5" dataDxfId="2"/>
+    <tableColumn id="14" name="R = FWHM/E" dataDxfId="1">
       <calculatedColumnFormula>K4/D4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0200-00000F000000}" name="dR" dataDxfId="0"/>
+    <tableColumn id="15" name="dR" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5910,14 +5953,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J203"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="7.7109375" customWidth="1"/>
     <col min="3" max="3" width="9.5703125" customWidth="1"/>
@@ -5927,8 +5970,8 @@
     <col min="7" max="7" width="7.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1"/>
-    <row r="2" spans="1:10" ht="44.1" thickBot="1">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -5951,7 +5994,7 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10" ht="15" thickBot="1">
+    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="152" t="s">
         <v>6</v>
       </c>
@@ -5971,7 +6014,7 @@
         <v>5.6333243243243238</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" s="229">
         <v>5.6360000000000001</v>
       </c>
@@ -5987,7 +6030,7 @@
       </c>
       <c r="G4" s="286"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" s="122">
         <v>6.2050000000000001</v>
       </c>
@@ -6001,7 +6044,7 @@
       </c>
       <c r="G5" s="124"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="122">
         <v>6.5869999999999997</v>
       </c>
@@ -6015,7 +6058,7 @@
       </c>
       <c r="G6" s="124"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" s="122">
         <v>7.1779999999999999</v>
       </c>
@@ -6029,7 +6072,7 @@
       </c>
       <c r="G7" s="124"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" s="117">
         <v>39.521999999999998</v>
       </c>
@@ -6043,7 +6086,7 @@
       </c>
       <c r="G8" s="125"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="117">
         <v>40.116999999999997</v>
       </c>
@@ -6057,7 +6100,7 @@
       </c>
       <c r="G9" s="125"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" s="224">
         <v>45.289000000000001</v>
       </c>
@@ -6074,7 +6117,7 @@
         <v>45.37024137931035</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" s="229">
         <v>45.412999999999997</v>
       </c>
@@ -6090,7 +6133,7 @@
       </c>
       <c r="G11" s="286"/>
     </row>
-    <row r="12" spans="1:10" ht="15" thickBot="1">
+    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="117">
         <v>46.578000000000003</v>
       </c>
@@ -6104,7 +6147,7 @@
       </c>
       <c r="G12" s="128"/>
     </row>
-    <row r="13" spans="1:10" ht="15" thickBot="1">
+    <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="153" t="s">
         <v>17</v>
       </c>
@@ -6119,7 +6162,7 @@
       <c r="F13" s="133"/>
       <c r="G13" s="134"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="135">
         <v>121.7817</v>
       </c>
@@ -6133,7 +6176,7 @@
       <c r="F14" s="133"/>
       <c r="G14" s="138"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="139">
         <v>125.68</v>
       </c>
@@ -6145,7 +6188,7 @@
       <c r="F15" s="133"/>
       <c r="G15" s="141"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="139">
         <v>137.56</v>
       </c>
@@ -6157,7 +6200,7 @@
       <c r="F16" s="133"/>
       <c r="G16" s="134"/>
     </row>
-    <row r="17" spans="2:7">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="139">
         <v>148</v>
       </c>
@@ -6169,7 +6212,7 @@
       <c r="F17" s="133"/>
       <c r="G17" s="142"/>
     </row>
-    <row r="18" spans="2:7">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="139">
         <v>150.13</v>
       </c>
@@ -6181,7 +6224,7 @@
       <c r="F18" s="133"/>
       <c r="G18" s="142"/>
     </row>
-    <row r="19" spans="2:7">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="139">
         <v>166.91</v>
       </c>
@@ -6193,7 +6236,7 @@
       <c r="F19" s="133"/>
       <c r="G19" s="142"/>
     </row>
-    <row r="20" spans="2:7">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="139">
         <v>172.1</v>
       </c>
@@ -6205,7 +6248,7 @@
       <c r="F20" s="133"/>
       <c r="G20" s="142"/>
     </row>
-    <row r="21" spans="2:7">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="139">
         <v>174.8</v>
       </c>
@@ -6217,7 +6260,7 @@
       <c r="F21" s="133"/>
       <c r="G21" s="142"/>
     </row>
-    <row r="22" spans="2:7">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="139">
         <v>175.18</v>
       </c>
@@ -6229,7 +6272,7 @@
       <c r="F22" s="133"/>
       <c r="G22" s="142"/>
     </row>
-    <row r="23" spans="2:7">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="139">
         <v>192.6</v>
       </c>
@@ -6241,7 +6284,7 @@
       <c r="F23" s="133"/>
       <c r="G23" s="142"/>
     </row>
-    <row r="24" spans="2:7">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="139">
         <v>195.22</v>
       </c>
@@ -6253,7 +6296,7 @@
       <c r="F24" s="133"/>
       <c r="G24" s="142"/>
     </row>
-    <row r="25" spans="2:7">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="139">
         <v>202.74</v>
       </c>
@@ -6265,7 +6308,7 @@
       <c r="F25" s="133"/>
       <c r="G25" s="142"/>
     </row>
-    <row r="26" spans="2:7">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="139">
         <v>207.03</v>
       </c>
@@ -6277,7 +6320,7 @@
       <c r="F26" s="133"/>
       <c r="G26" s="142"/>
     </row>
-    <row r="27" spans="2:7">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="139">
         <v>207.64</v>
       </c>
@@ -6289,7 +6332,7 @@
       <c r="F27" s="133"/>
       <c r="G27" s="142"/>
     </row>
-    <row r="28" spans="2:7">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="139">
         <v>209.3</v>
       </c>
@@ -6301,7 +6344,7 @@
       <c r="F28" s="133"/>
       <c r="G28" s="142"/>
     </row>
-    <row r="29" spans="2:7">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="139">
         <v>209.41</v>
       </c>
@@ -6313,7 +6356,7 @@
       <c r="F29" s="133"/>
       <c r="G29" s="142"/>
     </row>
-    <row r="30" spans="2:7">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="139">
         <v>209.97</v>
       </c>
@@ -6325,7 +6368,7 @@
       <c r="F30" s="133"/>
       <c r="G30" s="142"/>
     </row>
-    <row r="31" spans="2:7">
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="139">
         <v>210.95</v>
       </c>
@@ -6337,7 +6380,7 @@
       <c r="F31" s="133"/>
       <c r="G31" s="142"/>
     </row>
-    <row r="32" spans="2:7">
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="139">
         <v>212.43</v>
       </c>
@@ -6349,7 +6392,7 @@
       <c r="F32" s="133"/>
       <c r="G32" s="142"/>
     </row>
-    <row r="33" spans="2:7">
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="139">
         <v>237.1</v>
       </c>
@@ -6361,7 +6404,7 @@
       <c r="F33" s="133"/>
       <c r="G33" s="142"/>
     </row>
-    <row r="34" spans="2:7">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="139">
         <v>239.33</v>
       </c>
@@ -6373,7 +6416,7 @@
       <c r="F34" s="133"/>
       <c r="G34" s="142"/>
     </row>
-    <row r="35" spans="2:7">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="139">
         <v>241</v>
       </c>
@@ -6385,7 +6428,7 @@
       <c r="F35" s="133"/>
       <c r="G35" s="142"/>
     </row>
-    <row r="36" spans="2:7">
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="135">
         <v>244.69739999999999</v>
       </c>
@@ -6399,7 +6442,7 @@
       <c r="F36" s="133"/>
       <c r="G36" s="142"/>
     </row>
-    <row r="37" spans="2:7">
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="139">
         <v>251.63300000000001</v>
       </c>
@@ -6411,7 +6454,7 @@
       <c r="F37" s="133"/>
       <c r="G37" s="142"/>
     </row>
-    <row r="38" spans="2:7">
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B38" s="139">
         <v>269.83999999999997</v>
       </c>
@@ -6423,7 +6466,7 @@
       <c r="F38" s="133"/>
       <c r="G38" s="143"/>
     </row>
-    <row r="39" spans="2:7">
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B39" s="139">
         <v>271.08</v>
       </c>
@@ -6435,7 +6478,7 @@
       <c r="F39" s="133"/>
       <c r="G39" s="142"/>
     </row>
-    <row r="40" spans="2:7">
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B40" s="139">
         <v>272.41000000000003</v>
       </c>
@@ -6447,7 +6490,7 @@
       <c r="F40" s="133"/>
       <c r="G40" s="142"/>
     </row>
-    <row r="41" spans="2:7">
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B41" s="139">
         <v>275.42</v>
       </c>
@@ -6459,7 +6502,7 @@
       <c r="F41" s="133"/>
       <c r="G41" s="142"/>
     </row>
-    <row r="42" spans="2:7">
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B42" s="139">
         <v>285.98</v>
       </c>
@@ -6471,7 +6514,7 @@
       <c r="F42" s="133"/>
       <c r="G42" s="142"/>
     </row>
-    <row r="43" spans="2:7">
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B43" s="139">
         <v>286.5</v>
       </c>
@@ -6483,7 +6526,7 @@
       <c r="F43" s="133"/>
       <c r="G43" s="142"/>
     </row>
-    <row r="44" spans="2:7">
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B44" s="139">
         <v>287.10000000000002</v>
       </c>
@@ -6495,7 +6538,7 @@
       <c r="F44" s="133"/>
       <c r="G44" s="142"/>
     </row>
-    <row r="45" spans="2:7">
+    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B45" s="139">
         <v>295.93869999999998</v>
       </c>
@@ -6507,7 +6550,7 @@
       <c r="F45" s="133"/>
       <c r="G45" s="142"/>
     </row>
-    <row r="46" spans="2:7">
+    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B46" s="139">
         <v>315.10000000000002</v>
       </c>
@@ -6519,7 +6562,7 @@
       <c r="F46" s="133"/>
       <c r="G46" s="142"/>
     </row>
-    <row r="47" spans="2:7">
+    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B47" s="139">
         <v>316.13</v>
       </c>
@@ -6531,7 +6574,7 @@
       <c r="F47" s="133"/>
       <c r="G47" s="142"/>
     </row>
-    <row r="48" spans="2:7">
+    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B48" s="139">
         <v>320.10000000000002</v>
       </c>
@@ -6543,7 +6586,7 @@
       <c r="F48" s="133"/>
       <c r="G48" s="142"/>
     </row>
-    <row r="49" spans="2:7">
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="139">
         <v>324.83</v>
       </c>
@@ -6555,7 +6598,7 @@
       <c r="F49" s="133"/>
       <c r="G49" s="142"/>
     </row>
-    <row r="50" spans="2:7">
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="139">
         <v>324.91399999999999</v>
       </c>
@@ -6567,7 +6610,7 @@
       <c r="F50" s="133"/>
       <c r="G50" s="142"/>
     </row>
-    <row r="51" spans="2:7">
+    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B51" s="139">
         <v>328.76400000000001</v>
       </c>
@@ -6579,7 +6622,7 @@
       <c r="F51" s="133"/>
       <c r="G51" s="142"/>
     </row>
-    <row r="52" spans="2:7">
+    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B52" s="139">
         <v>329.41</v>
       </c>
@@ -6591,7 +6634,7 @@
       <c r="F52" s="133"/>
       <c r="G52" s="142"/>
     </row>
-    <row r="53" spans="2:7">
+    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B53" s="139">
         <v>330.58</v>
       </c>
@@ -6603,7 +6646,7 @@
       <c r="F53" s="133"/>
       <c r="G53" s="142"/>
     </row>
-    <row r="54" spans="2:7">
+    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B54" s="139">
         <v>340.46</v>
       </c>
@@ -6615,7 +6658,7 @@
       <c r="F54" s="133"/>
       <c r="G54" s="142"/>
     </row>
-    <row r="55" spans="2:7">
+    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B55" s="135">
         <v>344.27850000000001</v>
       </c>
@@ -6629,7 +6672,7 @@
       <c r="F55" s="133"/>
       <c r="G55" s="142"/>
     </row>
-    <row r="56" spans="2:7">
+    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B56" s="139">
         <v>345.54</v>
       </c>
@@ -6641,7 +6684,7 @@
       <c r="F56" s="133"/>
       <c r="G56" s="142"/>
     </row>
-    <row r="57" spans="2:7">
+    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B57" s="139">
         <v>348.75200000000001</v>
       </c>
@@ -6653,7 +6696,7 @@
       <c r="F57" s="133"/>
       <c r="G57" s="143"/>
     </row>
-    <row r="58" spans="2:7">
+    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B58" s="139">
         <v>351.66</v>
       </c>
@@ -6665,7 +6708,7 @@
       <c r="F58" s="133"/>
       <c r="G58" s="142"/>
     </row>
-    <row r="59" spans="2:7">
+    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B59" s="139">
         <v>354.16</v>
       </c>
@@ -6677,7 +6720,7 @@
       <c r="F59" s="133"/>
       <c r="G59" s="142"/>
     </row>
-    <row r="60" spans="2:7">
+    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B60" s="139">
         <v>357.26</v>
       </c>
@@ -6689,7 +6732,7 @@
       <c r="F60" s="133"/>
       <c r="G60" s="142"/>
     </row>
-    <row r="61" spans="2:7">
+    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B61" s="139">
         <v>358.48</v>
       </c>
@@ -6701,7 +6744,7 @@
       <c r="F61" s="133"/>
       <c r="G61" s="142"/>
     </row>
-    <row r="62" spans="2:7">
+    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B62" s="139">
         <v>367.78910000000002</v>
       </c>
@@ -6713,7 +6756,7 @@
       <c r="F62" s="133"/>
       <c r="G62" s="142"/>
     </row>
-    <row r="63" spans="2:7">
+    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B63" s="139">
         <v>378.15</v>
       </c>
@@ -6725,7 +6768,7 @@
       <c r="F63" s="133"/>
       <c r="G63" s="142"/>
     </row>
-    <row r="64" spans="2:7">
+    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B64" s="139">
         <v>379.36</v>
       </c>
@@ -6737,7 +6780,7 @@
       <c r="F64" s="133"/>
       <c r="G64" s="142"/>
     </row>
-    <row r="65" spans="2:7">
+    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B65" s="139">
         <v>385.61</v>
       </c>
@@ -6749,7 +6792,7 @@
       <c r="F65" s="133"/>
       <c r="G65" s="142"/>
     </row>
-    <row r="66" spans="2:7">
+    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B66" s="139">
         <v>387.9</v>
       </c>
@@ -6761,7 +6804,7 @@
       <c r="F66" s="133"/>
       <c r="G66" s="142"/>
     </row>
-    <row r="67" spans="2:7">
+    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B67" s="139">
         <v>389.07</v>
       </c>
@@ -6773,7 +6816,7 @@
       <c r="F67" s="133"/>
       <c r="G67" s="142"/>
     </row>
-    <row r="68" spans="2:7">
+    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B68" s="139">
         <v>391.19</v>
       </c>
@@ -6785,7 +6828,7 @@
       <c r="F68" s="133"/>
       <c r="G68" s="142"/>
     </row>
-    <row r="69" spans="2:7">
+    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B69" s="139">
         <v>395.75</v>
       </c>
@@ -6797,7 +6840,7 @@
       <c r="F69" s="133"/>
       <c r="G69" s="142"/>
     </row>
-    <row r="70" spans="2:7">
+    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B70" s="139">
         <v>397.75</v>
       </c>
@@ -6809,7 +6852,7 @@
       <c r="F70" s="133"/>
       <c r="G70" s="142"/>
     </row>
-    <row r="71" spans="2:7">
+    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B71" s="139">
         <v>401.29</v>
       </c>
@@ -6821,7 +6864,7 @@
       <c r="F71" s="133"/>
       <c r="G71" s="142"/>
     </row>
-    <row r="72" spans="2:7">
+    <row r="72" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B72" s="139">
         <v>406.74</v>
       </c>
@@ -6833,7 +6876,7 @@
       <c r="F72" s="133"/>
       <c r="G72" s="142"/>
     </row>
-    <row r="73" spans="2:7">
+    <row r="73" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B73" s="135">
         <v>411.11649999999997</v>
       </c>
@@ -6847,7 +6890,7 @@
       <c r="F73" s="133"/>
       <c r="G73" s="142"/>
     </row>
-    <row r="74" spans="2:7">
+    <row r="74" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B74" s="139">
         <v>416.02</v>
       </c>
@@ -6859,7 +6902,7 @@
       <c r="F74" s="133"/>
       <c r="G74" s="142"/>
     </row>
-    <row r="75" spans="2:7">
+    <row r="75" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B75" s="139">
         <v>423.45</v>
       </c>
@@ -6871,7 +6914,7 @@
       <c r="F75" s="133"/>
       <c r="G75" s="143"/>
     </row>
-    <row r="76" spans="2:7">
+    <row r="76" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B76" s="139">
         <v>440.86</v>
       </c>
@@ -6883,7 +6926,7 @@
       <c r="F76" s="133"/>
       <c r="G76" s="142"/>
     </row>
-    <row r="77" spans="2:7">
+    <row r="77" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B77" s="139">
         <v>441</v>
       </c>
@@ -6893,7 +6936,7 @@
       <c r="F77" s="133"/>
       <c r="G77" s="142"/>
     </row>
-    <row r="78" spans="2:7">
+    <row r="78" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B78" s="135">
         <v>443.9606</v>
       </c>
@@ -6907,7 +6950,7 @@
       <c r="F78" s="133"/>
       <c r="G78" s="142"/>
     </row>
-    <row r="79" spans="2:7">
+    <row r="79" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B79" s="139">
         <v>444.01</v>
       </c>
@@ -6919,7 +6962,7 @@
       <c r="F79" s="133"/>
       <c r="G79" s="142"/>
     </row>
-    <row r="80" spans="2:7">
+    <row r="80" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B80" s="139">
         <v>464.28</v>
       </c>
@@ -6931,7 +6974,7 @@
       <c r="F80" s="133"/>
       <c r="G80" s="143"/>
     </row>
-    <row r="81" spans="2:7">
+    <row r="81" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B81" s="139">
         <v>476.42</v>
       </c>
@@ -6943,7 +6986,7 @@
       <c r="F81" s="133"/>
       <c r="G81" s="142"/>
     </row>
-    <row r="82" spans="2:7">
+    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B82" s="139">
         <v>482.33</v>
       </c>
@@ -6955,7 +6998,7 @@
       <c r="F82" s="133"/>
       <c r="G82" s="142"/>
     </row>
-    <row r="83" spans="2:7">
+    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B83" s="139">
         <v>482.4</v>
       </c>
@@ -6967,7 +7010,7 @@
       <c r="F83" s="133"/>
       <c r="G83" s="142"/>
     </row>
-    <row r="84" spans="2:7">
+    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B84" s="139">
         <v>488.67919999999998</v>
       </c>
@@ -6979,7 +7022,7 @@
       <c r="F84" s="133"/>
       <c r="G84" s="142"/>
     </row>
-    <row r="85" spans="2:7">
+    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B85" s="139">
         <v>493.54</v>
       </c>
@@ -6991,7 +7034,7 @@
       <c r="F85" s="133"/>
       <c r="G85" s="142"/>
     </row>
-    <row r="86" spans="2:7">
+    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B86" s="139">
         <v>493.78</v>
       </c>
@@ -7003,7 +7046,7 @@
       <c r="F86" s="133"/>
       <c r="G86" s="142"/>
     </row>
-    <row r="87" spans="2:7">
+    <row r="87" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B87" s="139">
         <v>496.4</v>
       </c>
@@ -7015,7 +7058,7 @@
       <c r="F87" s="133"/>
       <c r="G87" s="142"/>
     </row>
-    <row r="88" spans="2:7">
+    <row r="88" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B88" s="139">
         <v>496.56</v>
       </c>
@@ -7027,7 +7070,7 @@
       <c r="F88" s="133"/>
       <c r="G88" s="142"/>
     </row>
-    <row r="89" spans="2:7">
+    <row r="89" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B89" s="139">
         <v>503.46699999999998</v>
       </c>
@@ -7039,7 +7082,7 @@
       <c r="F89" s="133"/>
       <c r="G89" s="142"/>
     </row>
-    <row r="90" spans="2:7">
+    <row r="90" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B90" s="139">
         <v>514.78</v>
       </c>
@@ -7051,7 +7094,7 @@
       <c r="F90" s="133"/>
       <c r="G90" s="142"/>
     </row>
-    <row r="91" spans="2:7">
+    <row r="91" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B91" s="139">
         <v>520.24</v>
       </c>
@@ -7063,7 +7106,7 @@
       <c r="F91" s="133"/>
       <c r="G91" s="142"/>
     </row>
-    <row r="92" spans="2:7">
+    <row r="92" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B92" s="139">
         <v>523.13</v>
       </c>
@@ -7075,7 +7118,7 @@
       <c r="F92" s="133"/>
       <c r="G92" s="142"/>
     </row>
-    <row r="93" spans="2:7">
+    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B93" s="139">
         <v>526.88</v>
       </c>
@@ -7087,7 +7130,7 @@
       <c r="F93" s="133"/>
       <c r="G93" s="142"/>
     </row>
-    <row r="94" spans="2:7">
+    <row r="94" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B94" s="139">
         <v>527.1</v>
       </c>
@@ -7099,7 +7142,7 @@
       <c r="F94" s="133"/>
       <c r="G94" s="142"/>
     </row>
-    <row r="95" spans="2:7">
+    <row r="95" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B95" s="139">
         <v>534.25</v>
       </c>
@@ -7111,7 +7154,7 @@
       <c r="F95" s="133"/>
       <c r="G95" s="142"/>
     </row>
-    <row r="96" spans="2:7">
+    <row r="96" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B96" s="139">
         <v>535.44000000000005</v>
       </c>
@@ -7123,7 +7166,7 @@
       <c r="F96" s="133"/>
       <c r="G96" s="142"/>
     </row>
-    <row r="97" spans="2:7">
+    <row r="97" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B97" s="139">
         <v>536.23</v>
       </c>
@@ -7133,7 +7176,7 @@
       <c r="F97" s="133"/>
       <c r="G97" s="142"/>
     </row>
-    <row r="98" spans="2:7">
+    <row r="98" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B98" s="139">
         <v>538.29</v>
       </c>
@@ -7145,7 +7188,7 @@
       <c r="F98" s="133"/>
       <c r="G98" s="142"/>
     </row>
-    <row r="99" spans="2:7">
+    <row r="99" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B99" s="139">
         <v>556.48</v>
       </c>
@@ -7157,7 +7200,7 @@
       <c r="F99" s="133"/>
       <c r="G99" s="142"/>
     </row>
-    <row r="100" spans="2:7">
+    <row r="100" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B100" s="139">
         <v>557.79999999999995</v>
       </c>
@@ -7169,7 +7212,7 @@
       <c r="F100" s="133"/>
       <c r="G100" s="142"/>
     </row>
-    <row r="101" spans="2:7">
+    <row r="101" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B101" s="139">
         <v>561.26</v>
       </c>
@@ -7181,7 +7224,7 @@
       <c r="F101" s="133"/>
       <c r="G101" s="142"/>
     </row>
-    <row r="102" spans="2:7">
+    <row r="102" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B102" s="139">
         <v>562.98</v>
       </c>
@@ -7193,7 +7236,7 @@
       <c r="F102" s="133"/>
       <c r="G102" s="142"/>
     </row>
-    <row r="103" spans="2:7">
+    <row r="103" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B103" s="139">
         <v>563.1</v>
       </c>
@@ -7205,7 +7248,7 @@
       <c r="F103" s="133"/>
       <c r="G103" s="142"/>
     </row>
-    <row r="104" spans="2:7">
+    <row r="104" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B104" s="139">
         <v>563.98599999999999</v>
       </c>
@@ -7217,7 +7260,7 @@
       <c r="F104" s="133"/>
       <c r="G104" s="142"/>
     </row>
-    <row r="105" spans="2:7">
+    <row r="105" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B105" s="139">
         <v>566.43799999999999</v>
       </c>
@@ -7229,7 +7272,7 @@
       <c r="F105" s="133"/>
       <c r="G105" s="142"/>
     </row>
-    <row r="106" spans="2:7">
+    <row r="106" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B106" s="139">
         <v>571.83000000000004</v>
       </c>
@@ -7241,7 +7284,7 @@
       <c r="F106" s="133"/>
       <c r="G106" s="142"/>
     </row>
-    <row r="107" spans="2:7">
+    <row r="107" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B107" s="139">
         <v>586.26480000000004</v>
       </c>
@@ -7253,7 +7296,7 @@
       <c r="F107" s="133"/>
       <c r="G107" s="142"/>
     </row>
-    <row r="108" spans="2:7">
+    <row r="108" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B108" s="139">
         <v>588.6</v>
       </c>
@@ -7265,7 +7308,7 @@
       <c r="F108" s="133"/>
       <c r="G108" s="142"/>
     </row>
-    <row r="109" spans="2:7">
+    <row r="109" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B109" s="139">
         <v>589.83000000000004</v>
       </c>
@@ -7277,7 +7320,7 @@
       <c r="F109" s="133"/>
       <c r="G109" s="142"/>
     </row>
-    <row r="110" spans="2:7">
+    <row r="110" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B110" s="139">
         <v>595.61</v>
       </c>
@@ -7289,7 +7332,7 @@
       <c r="F110" s="133"/>
       <c r="G110" s="142"/>
     </row>
-    <row r="111" spans="2:7">
+    <row r="111" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B111" s="139">
         <v>608.05999999999995</v>
       </c>
@@ -7301,7 +7344,7 @@
       <c r="F111" s="133"/>
       <c r="G111" s="142"/>
     </row>
-    <row r="112" spans="2:7">
+    <row r="112" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B112" s="139">
         <v>609.23</v>
       </c>
@@ -7313,7 +7356,7 @@
       <c r="F112" s="133"/>
       <c r="G112" s="142"/>
     </row>
-    <row r="113" spans="2:7">
+    <row r="113" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B113" s="139">
         <v>615.41</v>
       </c>
@@ -7323,7 +7366,7 @@
       <c r="F113" s="133"/>
       <c r="G113" s="142"/>
     </row>
-    <row r="114" spans="2:7">
+    <row r="114" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B114" s="139">
         <v>616.04999999999995</v>
       </c>
@@ -7335,7 +7378,7 @@
       <c r="F114" s="133"/>
       <c r="G114" s="142"/>
     </row>
-    <row r="115" spans="2:7">
+    <row r="115" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B115" s="139">
         <v>644.39</v>
       </c>
@@ -7347,7 +7390,7 @@
       <c r="F115" s="133"/>
       <c r="G115" s="142"/>
     </row>
-    <row r="116" spans="2:7">
+    <row r="116" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B116" s="139">
         <v>656.48900000000003</v>
       </c>
@@ -7359,7 +7402,7 @@
       <c r="F116" s="133"/>
       <c r="G116" s="142"/>
     </row>
-    <row r="117" spans="2:7">
+    <row r="117" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B117" s="139">
         <v>664.77</v>
       </c>
@@ -7371,7 +7414,7 @@
       <c r="F117" s="133"/>
       <c r="G117" s="142"/>
     </row>
-    <row r="118" spans="2:7">
+    <row r="118" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B118" s="139">
         <v>671.15499999999997</v>
       </c>
@@ -7383,7 +7426,7 @@
       <c r="F118" s="133"/>
       <c r="G118" s="142"/>
     </row>
-    <row r="119" spans="2:7">
+    <row r="119" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B119" s="139">
         <v>674.64</v>
       </c>
@@ -7395,7 +7438,7 @@
       <c r="F119" s="133"/>
       <c r="G119" s="142"/>
     </row>
-    <row r="120" spans="2:7">
+    <row r="120" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B120" s="139">
         <v>675</v>
       </c>
@@ -7407,7 +7450,7 @@
       <c r="F120" s="133"/>
       <c r="G120" s="142"/>
     </row>
-    <row r="121" spans="2:7">
+    <row r="121" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B121" s="139">
         <v>678.62300000000005</v>
       </c>
@@ -7419,7 +7462,7 @@
       <c r="F121" s="133"/>
       <c r="G121" s="142"/>
     </row>
-    <row r="122" spans="2:7">
+    <row r="122" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B122" s="139">
         <v>683.25</v>
       </c>
@@ -7431,7 +7474,7 @@
       <c r="F122" s="133"/>
       <c r="G122" s="142"/>
     </row>
-    <row r="123" spans="2:7">
+    <row r="123" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B123" s="139">
         <v>686.6</v>
       </c>
@@ -7443,7 +7486,7 @@
       <c r="F123" s="133"/>
       <c r="G123" s="142"/>
     </row>
-    <row r="124" spans="2:7">
+    <row r="124" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B124" s="139">
         <v>688.67</v>
       </c>
@@ -7455,7 +7498,7 @@
       <c r="F124" s="133"/>
       <c r="G124" s="142"/>
     </row>
-    <row r="125" spans="2:7">
+    <row r="125" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B125" s="139">
         <v>696.87</v>
       </c>
@@ -7467,7 +7510,7 @@
       <c r="F125" s="133"/>
       <c r="G125" s="142"/>
     </row>
-    <row r="126" spans="2:7">
+    <row r="126" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B126" s="139">
         <v>703.01</v>
       </c>
@@ -7479,7 +7522,7 @@
       <c r="F126" s="133"/>
       <c r="G126" s="142"/>
     </row>
-    <row r="127" spans="2:7">
+    <row r="127" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B127" s="139">
         <v>703.55</v>
       </c>
@@ -7491,7 +7534,7 @@
       <c r="F127" s="133"/>
       <c r="G127" s="142"/>
     </row>
-    <row r="128" spans="2:7">
+    <row r="128" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B128" s="139">
         <v>707.16</v>
       </c>
@@ -7503,7 +7546,7 @@
       <c r="F128" s="133"/>
       <c r="G128" s="142"/>
     </row>
-    <row r="129" spans="2:7">
+    <row r="129" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B129" s="139">
         <v>712.83</v>
       </c>
@@ -7515,7 +7558,7 @@
       <c r="F129" s="133"/>
       <c r="G129" s="142"/>
     </row>
-    <row r="130" spans="2:7">
+    <row r="130" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B130" s="139">
         <v>719.346</v>
       </c>
@@ -7527,7 +7570,7 @@
       <c r="F130" s="133"/>
       <c r="G130" s="142"/>
     </row>
-    <row r="131" spans="2:7">
+    <row r="131" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B131" s="139">
         <v>719.36</v>
       </c>
@@ -7539,7 +7582,7 @@
       <c r="F131" s="133"/>
       <c r="G131" s="142"/>
     </row>
-    <row r="132" spans="2:7">
+    <row r="132" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B132" s="139">
         <v>728.04</v>
       </c>
@@ -7551,7 +7594,7 @@
       <c r="F132" s="133"/>
       <c r="G132" s="142"/>
     </row>
-    <row r="133" spans="2:7">
+    <row r="133" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B133" s="139">
         <v>734.14</v>
       </c>
@@ -7563,7 +7606,7 @@
       <c r="F133" s="133"/>
       <c r="G133" s="142"/>
     </row>
-    <row r="134" spans="2:7">
+    <row r="134" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B134" s="139">
         <v>735.43</v>
       </c>
@@ -7575,7 +7618,7 @@
       <c r="F134" s="133"/>
       <c r="G134" s="142"/>
     </row>
-    <row r="135" spans="2:7">
+    <row r="135" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B135" s="139">
         <v>756.16</v>
       </c>
@@ -7587,7 +7630,7 @@
       <c r="F135" s="133"/>
       <c r="G135" s="142"/>
     </row>
-    <row r="136" spans="2:7">
+    <row r="136" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B136" s="139">
         <v>764.88</v>
       </c>
@@ -7599,7 +7642,7 @@
       <c r="F136" s="133"/>
       <c r="G136" s="142"/>
     </row>
-    <row r="137" spans="2:7">
+    <row r="137" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B137" s="139">
         <v>766.38</v>
       </c>
@@ -7611,7 +7654,7 @@
       <c r="F137" s="133"/>
       <c r="G137" s="142"/>
     </row>
-    <row r="138" spans="2:7">
+    <row r="138" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B138" s="139">
         <v>768.96</v>
       </c>
@@ -7623,7 +7666,7 @@
       <c r="F138" s="133"/>
       <c r="G138" s="142"/>
     </row>
-    <row r="139" spans="2:7">
+    <row r="139" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B139" s="135">
         <v>778.90449999999998</v>
       </c>
@@ -7637,7 +7680,7 @@
       <c r="F139" s="133"/>
       <c r="G139" s="142"/>
     </row>
-    <row r="140" spans="2:7">
+    <row r="140" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B140" s="139">
         <v>794.78</v>
       </c>
@@ -7649,7 +7692,7 @@
       <c r="F140" s="133"/>
       <c r="G140" s="142"/>
     </row>
-    <row r="141" spans="2:7">
+    <row r="141" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B141" s="139">
         <v>802</v>
       </c>
@@ -7661,7 +7704,7 @@
       <c r="F141" s="133"/>
       <c r="G141" s="143"/>
     </row>
-    <row r="142" spans="2:7">
+    <row r="142" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B142" s="139">
         <v>805.71</v>
       </c>
@@ -7673,7 +7716,7 @@
       <c r="F142" s="133"/>
       <c r="G142" s="142"/>
     </row>
-    <row r="143" spans="2:7">
+    <row r="143" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B143" s="139">
         <v>810.45100000000002</v>
       </c>
@@ -7685,7 +7728,7 @@
       <c r="F143" s="133"/>
       <c r="G143" s="142"/>
     </row>
-    <row r="144" spans="2:7">
+    <row r="144" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B144" s="139">
         <v>813.21</v>
       </c>
@@ -7697,7 +7740,7 @@
       <c r="F144" s="133"/>
       <c r="G144" s="142"/>
     </row>
-    <row r="145" spans="2:7">
+    <row r="145" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B145" s="139">
         <v>839.36</v>
       </c>
@@ -7709,7 +7752,7 @@
       <c r="F145" s="133"/>
       <c r="G145" s="142"/>
     </row>
-    <row r="146" spans="2:7">
+    <row r="146" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B146" s="139">
         <v>841.57399999999996</v>
       </c>
@@ -7721,7 +7764,7 @@
       <c r="F146" s="133"/>
       <c r="G146" s="142"/>
     </row>
-    <row r="147" spans="2:7">
+    <row r="147" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B147" s="139">
         <v>850.1</v>
       </c>
@@ -7733,7 +7776,7 @@
       <c r="F147" s="133"/>
       <c r="G147" s="142"/>
     </row>
-    <row r="148" spans="2:7">
+    <row r="148" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B148" s="139">
         <v>855.21</v>
       </c>
@@ -7745,7 +7788,7 @@
       <c r="F148" s="133"/>
       <c r="G148" s="142"/>
     </row>
-    <row r="149" spans="2:7">
+    <row r="149" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B149" s="135">
         <v>867.38</v>
       </c>
@@ -7759,7 +7802,7 @@
       <c r="F149" s="133"/>
       <c r="G149" s="142"/>
     </row>
-    <row r="150" spans="2:7">
+    <row r="150" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B150" s="139">
         <v>896.59</v>
       </c>
@@ -7771,7 +7814,7 @@
       <c r="F150" s="133"/>
       <c r="G150" s="142"/>
     </row>
-    <row r="151" spans="2:7">
+    <row r="151" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B151" s="139">
         <v>901.19</v>
       </c>
@@ -7783,7 +7826,7 @@
       <c r="F151" s="133"/>
       <c r="G151" s="143"/>
     </row>
-    <row r="152" spans="2:7">
+    <row r="152" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B152" s="139">
         <v>906.06</v>
       </c>
@@ -7795,7 +7838,7 @@
       <c r="F152" s="133"/>
       <c r="G152" s="142"/>
     </row>
-    <row r="153" spans="2:7">
+    <row r="153" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B153" s="139">
         <v>919.33699999999999</v>
       </c>
@@ -7807,7 +7850,7 @@
       <c r="F153" s="133"/>
       <c r="G153" s="142"/>
     </row>
-    <row r="154" spans="2:7">
+    <row r="154" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B154" s="139">
         <v>919.74</v>
       </c>
@@ -7819,7 +7862,7 @@
       <c r="F154" s="133"/>
       <c r="G154" s="142"/>
     </row>
-    <row r="155" spans="2:7">
+    <row r="155" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B155" s="139">
         <v>926.31</v>
       </c>
@@ -7831,7 +7874,7 @@
       <c r="F155" s="133"/>
       <c r="G155" s="142"/>
     </row>
-    <row r="156" spans="2:7">
+    <row r="156" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B156" s="139">
         <v>930.59</v>
       </c>
@@ -7843,7 +7886,7 @@
       <c r="F156" s="133"/>
       <c r="G156" s="142"/>
     </row>
-    <row r="157" spans="2:7">
+    <row r="157" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B157" s="139">
         <v>937.05</v>
       </c>
@@ -7855,7 +7898,7 @@
       <c r="F157" s="133"/>
       <c r="G157" s="142"/>
     </row>
-    <row r="158" spans="2:7">
+    <row r="158" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B158" s="139">
         <v>947.15</v>
       </c>
@@ -7867,7 +7910,7 @@
       <c r="F158" s="133"/>
       <c r="G158" s="142"/>
     </row>
-    <row r="159" spans="2:7">
+    <row r="159" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B159" s="139">
         <v>958.63</v>
       </c>
@@ -7879,7 +7922,7 @@
       <c r="F159" s="133"/>
       <c r="G159" s="142"/>
     </row>
-    <row r="160" spans="2:7">
+    <row r="160" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B160" s="139">
         <v>961.08</v>
       </c>
@@ -7891,7 +7934,7 @@
       <c r="F160" s="133"/>
       <c r="G160" s="142"/>
     </row>
-    <row r="161" spans="2:7">
+    <row r="161" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B161" s="139">
         <v>963.36699999999996</v>
       </c>
@@ -7903,7 +7946,7 @@
       <c r="F161" s="133"/>
       <c r="G161" s="142"/>
     </row>
-    <row r="162" spans="2:7">
+    <row r="162" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B162" s="135">
         <v>964.05700000000002</v>
       </c>
@@ -7917,7 +7960,7 @@
       <c r="F162" s="133"/>
       <c r="G162" s="142"/>
     </row>
-    <row r="163" spans="2:7">
+    <row r="163" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B163" s="139">
         <v>968.65</v>
       </c>
@@ -7929,7 +7972,7 @@
       <c r="F163" s="133"/>
       <c r="G163" s="142"/>
     </row>
-    <row r="164" spans="2:7">
+    <row r="164" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B164" s="139">
         <v>970.22</v>
       </c>
@@ -7941,7 +7984,7 @@
       <c r="F164" s="133"/>
       <c r="G164" s="143"/>
     </row>
-    <row r="165" spans="2:7">
+    <row r="165" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B165" s="139">
         <v>974.09</v>
       </c>
@@ -7953,7 +7996,7 @@
       <c r="F165" s="133"/>
       <c r="G165" s="142"/>
     </row>
-    <row r="166" spans="2:7">
+    <row r="166" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B166" s="139">
         <v>990.18</v>
       </c>
@@ -7965,7 +8008,7 @@
       <c r="F166" s="133"/>
       <c r="G166" s="142"/>
     </row>
-    <row r="167" spans="2:7">
+    <row r="167" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B167" s="139">
         <v>1001.1</v>
       </c>
@@ -7977,7 +8020,7 @@
       <c r="F167" s="133"/>
       <c r="G167" s="142"/>
     </row>
-    <row r="168" spans="2:7">
+    <row r="168" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B168" s="139">
         <v>1005.27</v>
       </c>
@@ -7989,7 +8032,7 @@
       <c r="F168" s="133"/>
       <c r="G168" s="142"/>
     </row>
-    <row r="169" spans="2:7">
+    <row r="169" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B169" s="139">
         <v>1050.0999999999999</v>
       </c>
@@ -8001,7 +8044,7 @@
       <c r="F169" s="133"/>
       <c r="G169" s="142"/>
     </row>
-    <row r="170" spans="2:7">
+    <row r="170" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B170" s="139">
         <v>1084</v>
       </c>
@@ -8013,7 +8056,7 @@
       <c r="F170" s="133"/>
       <c r="G170" s="142"/>
     </row>
-    <row r="171" spans="2:7">
+    <row r="171" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B171" s="139">
         <v>1084.3800000000001</v>
       </c>
@@ -8025,7 +8068,7 @@
       <c r="F171" s="133"/>
       <c r="G171" s="142"/>
     </row>
-    <row r="172" spans="2:7">
+    <row r="172" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B172" s="135">
         <v>1085.837</v>
       </c>
@@ -8039,7 +8082,7 @@
       <c r="F172" s="133"/>
       <c r="G172" s="142"/>
     </row>
-    <row r="173" spans="2:7">
+    <row r="173" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B173" s="135">
         <v>1089.7370000000001</v>
       </c>
@@ -8051,7 +8094,7 @@
       <c r="F173" s="133"/>
       <c r="G173" s="142"/>
     </row>
-    <row r="174" spans="2:7">
+    <row r="174" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B174" s="139">
         <v>1109.18</v>
       </c>
@@ -8063,7 +8106,7 @@
       <c r="F174" s="133"/>
       <c r="G174" s="143"/>
     </row>
-    <row r="175" spans="2:7">
+    <row r="175" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B175" s="135">
         <v>1112.076</v>
       </c>
@@ -8077,7 +8120,7 @@
       <c r="F175" s="133"/>
       <c r="G175" s="142"/>
     </row>
-    <row r="176" spans="2:7">
+    <row r="176" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B176" s="139">
         <v>1139</v>
       </c>
@@ -8089,7 +8132,7 @@
       <c r="F176" s="133"/>
       <c r="G176" s="142"/>
     </row>
-    <row r="177" spans="2:7">
+    <row r="177" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B177" s="139">
         <v>1170.97</v>
       </c>
@@ -8101,7 +8144,7 @@
       <c r="F177" s="133"/>
       <c r="G177" s="143"/>
     </row>
-    <row r="178" spans="2:7">
+    <row r="178" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B178" s="139">
         <v>1206.0899999999999</v>
       </c>
@@ -8113,7 +8156,7 @@
       <c r="F178" s="133"/>
       <c r="G178" s="142"/>
     </row>
-    <row r="179" spans="2:7">
+    <row r="179" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B179" s="144">
         <v>1212.9480000000001</v>
       </c>
@@ -8125,7 +8168,7 @@
       <c r="F179" s="133"/>
       <c r="G179" s="142"/>
     </row>
-    <row r="180" spans="2:7">
+    <row r="180" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B180" s="144">
         <v>1246.3399999999999</v>
       </c>
@@ -8137,7 +8180,7 @@
       <c r="F180" s="133"/>
       <c r="G180" s="142"/>
     </row>
-    <row r="181" spans="2:7">
+    <row r="181" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B181" s="144">
         <v>1249.94</v>
       </c>
@@ -8149,7 +8192,7 @@
       <c r="F181" s="133"/>
       <c r="G181" s="142"/>
     </row>
-    <row r="182" spans="2:7">
+    <row r="182" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B182" s="144">
         <v>1261.3499999999999</v>
       </c>
@@ -8161,7 +8204,7 @@
       <c r="F182" s="133"/>
       <c r="G182" s="142"/>
     </row>
-    <row r="183" spans="2:7">
+    <row r="183" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B183" s="144">
         <v>1292.78</v>
       </c>
@@ -8173,7 +8216,7 @@
       <c r="F183" s="133"/>
       <c r="G183" s="142"/>
     </row>
-    <row r="184" spans="2:7">
+    <row r="184" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B184" s="144">
         <v>1299.1420000000001</v>
       </c>
@@ -8185,7 +8228,7 @@
       <c r="F184" s="133"/>
       <c r="G184" s="142"/>
     </row>
-    <row r="185" spans="2:7">
+    <row r="185" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B185" s="144">
         <v>1314.6</v>
       </c>
@@ -8197,7 +8240,7 @@
       <c r="F185" s="133"/>
       <c r="G185" s="142"/>
     </row>
-    <row r="186" spans="2:7">
+    <row r="186" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B186" s="144">
         <v>1315.58</v>
       </c>
@@ -8209,7 +8252,7 @@
       <c r="F186" s="133"/>
       <c r="G186" s="142"/>
     </row>
-    <row r="187" spans="2:7">
+    <row r="187" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B187" s="144">
         <v>1318.38</v>
       </c>
@@ -8221,7 +8264,7 @@
       <c r="F187" s="133"/>
       <c r="G187" s="142"/>
     </row>
-    <row r="188" spans="2:7">
+    <row r="188" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B188" s="144">
         <v>1348.1</v>
       </c>
@@ -8233,7 +8276,7 @@
       <c r="F188" s="133"/>
       <c r="G188" s="142"/>
     </row>
-    <row r="189" spans="2:7">
+    <row r="189" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B189" s="144">
         <v>1363.78</v>
       </c>
@@ -8245,7 +8288,7 @@
       <c r="F189" s="133"/>
       <c r="G189" s="142"/>
     </row>
-    <row r="190" spans="2:7">
+    <row r="190" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B190" s="144">
         <v>1390.5</v>
       </c>
@@ -8257,7 +8300,7 @@
       <c r="F190" s="133"/>
       <c r="G190" s="142"/>
     </row>
-    <row r="191" spans="2:7">
+    <row r="191" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B191" s="144">
         <v>1408.0129999999999</v>
       </c>
@@ -8269,7 +8312,7 @@
       <c r="F191" s="133"/>
       <c r="G191" s="142"/>
     </row>
-    <row r="192" spans="2:7">
+    <row r="192" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B192" s="139">
         <v>1455.1</v>
       </c>
@@ -8281,7 +8324,7 @@
       <c r="F192" s="133"/>
       <c r="G192" s="142"/>
     </row>
-    <row r="193" spans="2:7">
+    <row r="193" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B193" s="139">
         <v>1457.643</v>
       </c>
@@ -8293,7 +8336,7 @@
       <c r="F193" s="133"/>
       <c r="G193" s="142"/>
     </row>
-    <row r="194" spans="2:7">
+    <row r="194" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B194" s="139">
         <v>1485.9</v>
       </c>
@@ -8305,7 +8348,7 @@
       <c r="F194" s="133"/>
       <c r="G194" s="142"/>
     </row>
-    <row r="195" spans="2:7">
+    <row r="195" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B195" s="139">
         <v>1491.4</v>
       </c>
@@ -8317,7 +8360,7 @@
       <c r="F195" s="133"/>
       <c r="G195" s="142"/>
     </row>
-    <row r="196" spans="2:7">
+    <row r="196" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B196" s="139">
         <v>1528.1</v>
       </c>
@@ -8329,7 +8372,7 @@
       <c r="F196" s="133"/>
       <c r="G196" s="142"/>
     </row>
-    <row r="197" spans="2:7">
+    <row r="197" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B197" s="139">
         <v>1605.62</v>
       </c>
@@ -8341,7 +8384,7 @@
       <c r="F197" s="133"/>
       <c r="G197" s="142"/>
     </row>
-    <row r="198" spans="2:7">
+    <row r="198" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B198" s="139">
         <v>1608.36</v>
       </c>
@@ -8353,7 +8396,7 @@
       <c r="F198" s="133"/>
       <c r="G198" s="142"/>
     </row>
-    <row r="199" spans="2:7">
+    <row r="199" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B199" s="139">
         <v>1635.38</v>
       </c>
@@ -8365,7 +8408,7 @@
       <c r="F199" s="133"/>
       <c r="G199" s="142"/>
     </row>
-    <row r="200" spans="2:7">
+    <row r="200" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B200" s="139">
         <v>1647.44</v>
       </c>
@@ -8377,7 +8420,7 @@
       <c r="F200" s="133"/>
       <c r="G200" s="142"/>
     </row>
-    <row r="201" spans="2:7">
+    <row r="201" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B201" s="139">
         <v>1674.31</v>
       </c>
@@ -8389,7 +8432,7 @@
       <c r="F201" s="133"/>
       <c r="G201" s="142"/>
     </row>
-    <row r="202" spans="2:7">
+    <row r="202" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B202" s="139">
         <v>1698.1</v>
       </c>
@@ -8401,7 +8444,7 @@
       <c r="F202" s="133"/>
       <c r="G202" s="142"/>
     </row>
-    <row r="203" spans="2:7" ht="15" thickBot="1">
+    <row r="203" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B203" s="146">
         <v>1769.09</v>
       </c>
@@ -8427,21 +8470,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B10" sqref="B10:G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="9.5703125" customWidth="1"/>
     <col min="7" max="7" width="7.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1"/>
-    <row r="2" spans="1:7" ht="47.1" thickBot="1">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:7" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -8461,7 +8504,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1">
+    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="152" t="s">
         <v>6</v>
       </c>
@@ -8481,7 +8524,7 @@
         <v>4.2846126126126123</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="122">
         <v>4.2859999999999996</v>
       </c>
@@ -8497,7 +8540,7 @@
       </c>
       <c r="G4" s="288"/>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="122">
         <v>4.6189999999999998</v>
       </c>
@@ -8511,7 +8554,7 @@
       </c>
       <c r="G5" s="168"/>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" s="122">
         <v>4.9359999999999999</v>
       </c>
@@ -8525,7 +8568,7 @@
       </c>
       <c r="G6" s="168"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="122">
         <v>5.28</v>
       </c>
@@ -8539,7 +8582,7 @@
       </c>
       <c r="G7" s="168"/>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="246">
         <v>30.625</v>
       </c>
@@ -8553,7 +8596,7 @@
       </c>
       <c r="G8" s="291"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" s="251">
         <v>30.972999999999999</v>
       </c>
@@ -8567,7 +8610,7 @@
       </c>
       <c r="G9" s="292"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" s="246">
         <v>34.918999999999997</v>
       </c>
@@ -8586,7 +8629,7 @@
         <v>34.964333333333336</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" s="122">
         <v>34.987000000000002</v>
       </c>
@@ -8602,7 +8645,7 @@
       <c r="F11" s="121"/>
       <c r="G11" s="288"/>
     </row>
-    <row r="12" spans="1:7" ht="15" thickBot="1">
+    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="248">
         <v>35.822000000000003</v>
       </c>
@@ -8616,7 +8659,7 @@
       </c>
       <c r="G12" s="171"/>
     </row>
-    <row r="13" spans="1:7" ht="15" thickBot="1">
+    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="154" t="s">
         <v>17</v>
       </c>
@@ -8633,7 +8676,7 @@
       <c r="F13" s="159"/>
       <c r="G13" s="169"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" s="240">
         <v>79.614199999999997</v>
       </c>
@@ -8645,7 +8688,7 @@
       <c r="F14" s="244"/>
       <c r="G14" s="245"/>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" s="234">
         <v>80.997900000000001</v>
       </c>
@@ -8659,7 +8702,7 @@
       <c r="F15" s="238"/>
       <c r="G15" s="239"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" s="160">
         <v>160.61199999999999</v>
       </c>
@@ -8671,7 +8714,7 @@
       <c r="F16" s="159"/>
       <c r="G16" s="169"/>
     </row>
-    <row r="17" spans="2:7">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="160">
         <v>223.23679999999999</v>
       </c>
@@ -8683,7 +8726,7 @@
       <c r="F17" s="159"/>
       <c r="G17" s="169"/>
     </row>
-    <row r="18" spans="2:7">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="160">
         <v>276.39890000000003</v>
       </c>
@@ -8697,7 +8740,7 @@
       <c r="F18" s="159"/>
       <c r="G18" s="169"/>
     </row>
-    <row r="19" spans="2:7">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="160">
         <v>302.85079999999999</v>
       </c>
@@ -8711,7 +8754,7 @@
       <c r="F19" s="159"/>
       <c r="G19" s="169"/>
     </row>
-    <row r="20" spans="2:7">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="160">
         <v>356.0129</v>
       </c>
@@ -8725,7 +8768,7 @@
       <c r="F20" s="159"/>
       <c r="G20" s="169"/>
     </row>
-    <row r="21" spans="2:7" ht="15" thickBot="1">
+    <row r="21" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="163">
         <v>383.8485</v>
       </c>
@@ -8752,20 +8795,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1"/>
-    <row r="2" spans="1:6" ht="31.5" thickBot="1">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -8782,7 +8825,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" thickBot="1">
+    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="152" t="s">
         <v>6</v>
       </c>
@@ -8798,7 +8841,7 @@
       <c r="E3" s="116"/>
       <c r="F3" s="182"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" s="180">
         <v>31.815999999999999</v>
       </c>
@@ -8814,7 +8857,7 @@
         <v>32.060360902255638</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" s="180">
         <v>32.192999999999998</v>
       </c>
@@ -8827,7 +8870,7 @@
       <c r="E5" s="293"/>
       <c r="F5" s="124"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" s="180">
         <v>36.481999999999999</v>
       </c>
@@ -8843,7 +8886,7 @@
         <v>36.732293929712462</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" s="180">
         <v>36.826999999999998</v>
       </c>
@@ -8856,7 +8899,7 @@
       <c r="E7" s="293"/>
       <c r="F7" s="124"/>
     </row>
-    <row r="8" spans="1:6" ht="15" thickBot="1">
+    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="180">
         <v>37.255000000000003</v>
       </c>
@@ -8869,7 +8912,7 @@
       <c r="E8" s="121"/>
       <c r="F8" s="171"/>
     </row>
-    <row r="9" spans="1:6" ht="15" thickBot="1">
+    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="154" t="s">
         <v>17</v>
       </c>
@@ -8883,7 +8926,7 @@
       <c r="E9" s="177"/>
       <c r="F9" s="183"/>
     </row>
-    <row r="10" spans="1:6" ht="15" thickBot="1">
+    <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="173">
         <v>661.65700000000004</v>
       </c>
@@ -8907,19 +8950,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="31.5" thickBot="1">
+    <row r="2" spans="1:5" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -8933,7 +8976,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15" thickBot="1">
+    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="152" t="s">
         <v>6</v>
       </c>
@@ -8948,7 +8991,7 @@
       </c>
       <c r="E3" s="203"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" s="204">
         <v>7.4610000000000003</v>
       </c>
@@ -8960,7 +9003,7 @@
       </c>
       <c r="E4" s="207"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" s="204">
         <v>7.4779999999999998</v>
       </c>
@@ -8972,7 +9015,7 @@
       </c>
       <c r="E5" s="207"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="204">
         <v>8.2959999999999994</v>
       </c>
@@ -8984,7 +9027,7 @@
       </c>
       <c r="E6" s="207"/>
     </row>
-    <row r="7" spans="1:5" ht="15" thickBot="1">
+    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="208">
         <v>8.2959999999999994</v>
       </c>
@@ -8996,7 +9039,7 @@
       </c>
       <c r="E7" s="211"/>
     </row>
-    <row r="8" spans="1:5" ht="15" thickBot="1">
+    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="154" t="s">
         <v>17</v>
       </c>
@@ -9009,7 +9052,7 @@
       <c r="D8" s="187"/>
       <c r="E8" s="188"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="189">
         <v>826.1</v>
       </c>
@@ -9019,7 +9062,7 @@
       <c r="D9" s="191"/>
       <c r="E9" s="188"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" s="192">
         <v>1173.2280000000001</v>
       </c>
@@ -9031,7 +9074,7 @@
         <v>3638</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" s="189">
         <v>1332.492</v>
       </c>
@@ -9041,7 +9084,7 @@
       <c r="D11" s="191"/>
       <c r="E11" s="188"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" s="189">
         <v>2158.5700000000002</v>
       </c>
@@ -9051,7 +9094,7 @@
       <c r="D12" s="191"/>
       <c r="E12" s="188"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" s="196">
         <v>2505.692</v>
       </c>
@@ -9068,14 +9111,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G50"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="C2" sqref="C2:F50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="9.5703125" customWidth="1"/>
     <col min="5" max="5" width="10.85546875" customWidth="1"/>
@@ -9083,7 +9126,7 @@
     <col min="7" max="7" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" ht="30.95">
+    <row r="2" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C2" s="212" t="s">
         <v>0</v>
       </c>
@@ -9100,7 +9143,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:7">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="26"/>
       <c r="C3" s="216">
         <f t="shared" ref="C3:C50" si="0">F3*0.3225-0.0825</f>
@@ -9115,7 +9158,7 @@
       </c>
       <c r="G3" s="20"/>
     </row>
-    <row r="4" spans="2:7">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C4" s="217">
         <f t="shared" si="0"/>
         <v>27.6525</v>
@@ -9129,7 +9172,7 @@
       </c>
       <c r="G4" s="22"/>
     </row>
-    <row r="5" spans="2:7">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C5" s="217">
         <f t="shared" si="0"/>
         <v>47.002499999999998</v>
@@ -9143,7 +9186,7 @@
       </c>
       <c r="G5" s="22"/>
     </row>
-    <row r="6" spans="2:7">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C6" s="217">
         <f t="shared" si="0"/>
         <v>59.58</v>
@@ -9157,7 +9200,7 @@
       </c>
       <c r="G6" s="22"/>
     </row>
-    <row r="7" spans="2:7">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C7" s="217">
         <f t="shared" si="0"/>
         <v>63.772500000000001</v>
@@ -9171,7 +9214,7 @@
       </c>
       <c r="G7" s="22"/>
     </row>
-    <row r="8" spans="2:7">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="26"/>
       <c r="C8" s="217">
         <f t="shared" si="0"/>
@@ -9186,7 +9229,7 @@
       </c>
       <c r="G8" s="22"/>
     </row>
-    <row r="9" spans="2:7">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C9" s="217">
         <f t="shared" si="0"/>
         <v>77.31750000000001</v>
@@ -9200,7 +9243,7 @@
       </c>
       <c r="G9" s="22"/>
     </row>
-    <row r="10" spans="2:7">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C10" s="217">
         <f t="shared" si="0"/>
         <v>84.412500000000009</v>
@@ -9214,7 +9257,7 @@
       </c>
       <c r="G10" s="22"/>
     </row>
-    <row r="11" spans="2:7">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C11" s="217">
         <f t="shared" si="0"/>
         <v>87.637500000000003</v>
@@ -9228,7 +9271,7 @@
       </c>
       <c r="G11" s="22"/>
     </row>
-    <row r="12" spans="2:7">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C12" s="217">
         <f t="shared" si="0"/>
         <v>90.217500000000001</v>
@@ -9242,7 +9285,7 @@
       </c>
       <c r="G12" s="22"/>
     </row>
-    <row r="13" spans="2:7">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C13" s="218">
         <f t="shared" si="0"/>
         <v>93.12</v>
@@ -9256,7 +9299,7 @@
       </c>
       <c r="G13" s="25"/>
     </row>
-    <row r="14" spans="2:7">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C14" s="217">
         <f t="shared" si="0"/>
         <v>144.39750000000001</v>
@@ -9268,7 +9311,7 @@
       </c>
       <c r="G14" s="22"/>
     </row>
-    <row r="15" spans="2:7">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C15" s="217">
         <f t="shared" si="0"/>
         <v>186.32249999999999</v>
@@ -9282,7 +9325,7 @@
       </c>
       <c r="G15" s="22"/>
     </row>
-    <row r="16" spans="2:7">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C16" s="217">
         <f t="shared" si="0"/>
         <v>209.86500000000001</v>
@@ -9294,7 +9337,7 @@
       </c>
       <c r="G16" s="22"/>
     </row>
-    <row r="17" spans="3:7">
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C17" s="217">
         <f t="shared" si="0"/>
         <v>238.89</v>
@@ -9310,7 +9353,7 @@
       </c>
       <c r="G17" s="22"/>
     </row>
-    <row r="18" spans="3:7">
+    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C18" s="217">
         <f t="shared" si="0"/>
         <v>242.11500000000001</v>
@@ -9326,7 +9369,7 @@
       </c>
       <c r="G18" s="22"/>
     </row>
-    <row r="19" spans="3:7">
+    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C19" s="217">
         <f t="shared" si="0"/>
         <v>270.495</v>
@@ -9338,7 +9381,7 @@
       </c>
       <c r="G19" s="22"/>
     </row>
-    <row r="20" spans="3:7">
+    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C20" s="217">
         <f t="shared" si="0"/>
         <v>295.32750000000004</v>
@@ -9354,7 +9397,7 @@
       </c>
       <c r="G20" s="22"/>
     </row>
-    <row r="21" spans="3:7">
+    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C21" s="217">
         <f t="shared" si="0"/>
         <v>300.16500000000002</v>
@@ -9370,7 +9413,7 @@
       </c>
       <c r="G21" s="22"/>
     </row>
-    <row r="22" spans="3:7">
+    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C22" s="217">
         <f t="shared" si="0"/>
         <v>338.54250000000002</v>
@@ -9382,7 +9425,7 @@
       </c>
       <c r="G22" s="22"/>
     </row>
-    <row r="23" spans="3:7">
+    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C23" s="217">
         <f t="shared" si="0"/>
         <v>352.08750000000003</v>
@@ -9398,7 +9441,7 @@
       </c>
       <c r="G23" s="22"/>
     </row>
-    <row r="24" spans="3:7">
+    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C24" s="217">
         <f t="shared" si="0"/>
         <v>409.49250000000001</v>
@@ -9410,7 +9453,7 @@
       </c>
       <c r="G24" s="22"/>
     </row>
-    <row r="25" spans="3:7">
+    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C25" s="217">
         <f t="shared" si="0"/>
         <v>462.70500000000004</v>
@@ -9422,7 +9465,7 @@
       </c>
       <c r="G25" s="22"/>
     </row>
-    <row r="26" spans="3:7">
+    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C26" s="217">
         <f t="shared" si="0"/>
         <v>481.08750000000003</v>
@@ -9434,7 +9477,7 @@
       </c>
       <c r="G26" s="22"/>
     </row>
-    <row r="27" spans="3:7">
+    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C27" s="219">
         <f t="shared" si="0"/>
         <v>511.08000000000004</v>
@@ -9446,7 +9489,7 @@
       </c>
       <c r="G27" s="22"/>
     </row>
-    <row r="28" spans="3:7">
+    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C28" s="217">
         <f t="shared" si="0"/>
         <v>533.97750000000008</v>
@@ -9458,7 +9501,7 @@
       </c>
       <c r="G28" s="22"/>
     </row>
-    <row r="29" spans="3:7">
+    <row r="29" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C29" s="217">
         <f t="shared" si="0"/>
         <v>570.09750000000008</v>
@@ -9472,7 +9515,7 @@
       </c>
       <c r="G29" s="22"/>
     </row>
-    <row r="30" spans="3:7">
+    <row r="30" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C30" s="217">
         <f t="shared" si="0"/>
         <v>583.32000000000005</v>
@@ -9488,7 +9531,7 @@
       </c>
       <c r="G30" s="22"/>
     </row>
-    <row r="31" spans="3:7">
+    <row r="31" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C31" s="217">
         <f t="shared" si="0"/>
         <v>609.4425</v>
@@ -9504,7 +9547,7 @@
       </c>
       <c r="G31" s="22"/>
     </row>
-    <row r="32" spans="3:7">
+    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C32" s="217">
         <f t="shared" si="0"/>
         <v>665.5575</v>
@@ -9520,7 +9563,7 @@
       </c>
       <c r="G32" s="22"/>
     </row>
-    <row r="33" spans="3:7">
+    <row r="33" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C33" s="217">
         <f t="shared" si="0"/>
         <v>727.15500000000009</v>
@@ -9536,7 +9579,7 @@
       </c>
       <c r="G33" s="22"/>
     </row>
-    <row r="34" spans="3:7">
+    <row r="34" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C34" s="217">
         <f t="shared" si="0"/>
         <v>768.75750000000005</v>
@@ -9552,7 +9595,7 @@
       </c>
       <c r="G34" s="22"/>
     </row>
-    <row r="35" spans="3:7">
+    <row r="35" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C35" s="217">
         <f t="shared" si="0"/>
         <v>784.88250000000005</v>
@@ -9568,7 +9611,7 @@
       </c>
       <c r="G35" s="22"/>
     </row>
-    <row r="36" spans="3:7">
+    <row r="36" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C36" s="217">
         <f t="shared" si="0"/>
         <v>794.88</v>
@@ -9580,7 +9623,7 @@
       </c>
       <c r="G36" s="22"/>
     </row>
-    <row r="37" spans="3:7">
+    <row r="37" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C37" s="217">
         <f t="shared" si="0"/>
         <v>806.16750000000002</v>
@@ -9596,7 +9639,7 @@
       </c>
       <c r="G37" s="22"/>
     </row>
-    <row r="38" spans="3:7">
+    <row r="38" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C38" s="217">
         <f t="shared" si="0"/>
         <v>839.38499999999999</v>
@@ -9608,7 +9651,7 @@
       </c>
       <c r="G38" s="22"/>
     </row>
-    <row r="39" spans="3:7">
+    <row r="39" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C39" s="217">
         <f t="shared" si="0"/>
         <v>860.99250000000006</v>
@@ -9624,7 +9667,7 @@
       </c>
       <c r="G39" s="22"/>
     </row>
-    <row r="40" spans="3:7">
+    <row r="40" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C40" s="217">
         <f t="shared" si="0"/>
         <v>911.30250000000001</v>
@@ -9636,7 +9679,7 @@
       </c>
       <c r="G40" s="22"/>
     </row>
-    <row r="41" spans="3:7">
+    <row r="41" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C41" s="217">
         <f t="shared" si="0"/>
         <v>934.2</v>
@@ -9652,7 +9695,7 @@
       </c>
       <c r="G41" s="22"/>
     </row>
-    <row r="42" spans="3:7">
+    <row r="42" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C42" s="217">
         <f t="shared" si="0"/>
         <v>964.83750000000009</v>
@@ -9666,7 +9709,7 @@
       </c>
       <c r="G42" s="22"/>
     </row>
-    <row r="43" spans="3:7">
+    <row r="43" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C43" s="217">
         <f t="shared" si="0"/>
         <v>968.7075000000001</v>
@@ -9678,7 +9721,7 @@
       </c>
       <c r="G43" s="22"/>
     </row>
-    <row r="44" spans="3:7">
+    <row r="44" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C44" s="217">
         <f t="shared" si="0"/>
         <v>1001.2800000000001</v>
@@ -9694,7 +9737,7 @@
       </c>
       <c r="G44" s="22"/>
     </row>
-    <row r="45" spans="3:7">
+    <row r="45" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C45" s="217">
         <f t="shared" si="0"/>
         <v>1051.9125000000001</v>
@@ -9706,7 +9749,7 @@
       </c>
       <c r="G45" s="22"/>
     </row>
-    <row r="46" spans="3:7">
+    <row r="46" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C46" s="217">
         <f t="shared" si="0"/>
         <v>1069.9725000000001</v>
@@ -9718,7 +9761,7 @@
       </c>
       <c r="G46" s="22"/>
     </row>
-    <row r="47" spans="3:7">
+    <row r="47" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C47" s="217">
         <f t="shared" si="0"/>
         <v>1120.605</v>
@@ -9734,7 +9777,7 @@
       </c>
       <c r="G47" s="22"/>
     </row>
-    <row r="48" spans="3:7">
+    <row r="48" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C48" s="217">
         <f t="shared" si="0"/>
         <v>1155.4349999999999</v>
@@ -9750,7 +9793,7 @@
       </c>
       <c r="G48" s="22"/>
     </row>
-    <row r="49" spans="3:7">
+    <row r="49" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C49" s="217">
         <f t="shared" si="0"/>
         <v>1238.6400000000001</v>
@@ -9766,7 +9809,7 @@
       </c>
       <c r="G49" s="22"/>
     </row>
-    <row r="50" spans="3:7">
+    <row r="50" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C50" s="218">
         <f t="shared" si="0"/>
         <v>1280.8875</v>
@@ -9789,14 +9832,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I36"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="7" customWidth="1"/>
     <col min="3" max="3" width="8.140625" customWidth="1"/>
@@ -9808,7 +9851,7 @@
     <col min="9" max="9" width="7.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" ht="44.1" thickBot="1">
+    <row r="2" spans="2:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="259" t="s">
         <v>49</v>
       </c>
@@ -9834,7 +9877,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="2:9">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="263" t="s">
         <v>53</v>
       </c>
@@ -9856,7 +9899,7 @@
       <c r="H3" s="31"/>
       <c r="I3" s="32"/>
     </row>
-    <row r="4" spans="2:9">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="30" t="s">
         <v>57</v>
       </c>
@@ -9878,7 +9921,7 @@
       <c r="H4" s="10"/>
       <c r="I4" s="30"/>
     </row>
-    <row r="5" spans="2:9">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="30" t="s">
         <v>57</v>
       </c>
@@ -9900,7 +9943,7 @@
       <c r="H5" s="10"/>
       <c r="I5" s="30"/>
     </row>
-    <row r="6" spans="2:9">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="30" t="s">
         <v>57</v>
       </c>
@@ -9920,7 +9963,7 @@
       <c r="H6" s="10"/>
       <c r="I6" s="30"/>
     </row>
-    <row r="7" spans="2:9">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="30" t="s">
         <v>57</v>
       </c>
@@ -9942,7 +9985,7 @@
       <c r="H7" s="10"/>
       <c r="I7" s="30"/>
     </row>
-    <row r="8" spans="2:9">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="30" t="s">
         <v>57</v>
       </c>
@@ -9964,7 +10007,7 @@
       <c r="H8" s="10"/>
       <c r="I8" s="30"/>
     </row>
-    <row r="9" spans="2:9" ht="29.1">
+    <row r="9" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="30" t="s">
         <v>57</v>
       </c>
@@ -9986,7 +10029,7 @@
       <c r="H9" s="10"/>
       <c r="I9" s="30"/>
     </row>
-    <row r="10" spans="2:9">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="30" t="s">
         <v>57</v>
       </c>
@@ -10008,7 +10051,7 @@
       <c r="H10" s="10"/>
       <c r="I10" s="30"/>
     </row>
-    <row r="11" spans="2:9">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="30" t="s">
         <v>57</v>
       </c>
@@ -10032,7 +10075,7 @@
       </c>
       <c r="I11" s="33"/>
     </row>
-    <row r="12" spans="2:9">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="30" t="s">
         <v>57</v>
       </c>
@@ -10056,7 +10099,7 @@
       </c>
       <c r="I12" s="33"/>
     </row>
-    <row r="13" spans="2:9">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="30" t="s">
         <v>57</v>
       </c>
@@ -10080,7 +10123,7 @@
       </c>
       <c r="I13" s="33"/>
     </row>
-    <row r="14" spans="2:9">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="30" t="s">
         <v>57</v>
       </c>
@@ -10104,7 +10147,7 @@
       </c>
       <c r="I14" s="33"/>
     </row>
-    <row r="15" spans="2:9" ht="15" thickBot="1">
+    <row r="15" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="35" t="s">
         <v>57</v>
       </c>
@@ -10128,7 +10171,7 @@
       </c>
       <c r="I15" s="33"/>
     </row>
-    <row r="16" spans="2:9">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="264" t="s">
         <v>47</v>
       </c>
@@ -10150,7 +10193,7 @@
       <c r="H16" s="31"/>
       <c r="I16" s="32"/>
     </row>
-    <row r="17" spans="2:9">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="30" t="s">
         <v>57</v>
       </c>
@@ -10172,7 +10215,7 @@
       <c r="H17" s="10"/>
       <c r="I17" s="30"/>
     </row>
-    <row r="18" spans="2:9">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="30" t="s">
         <v>57</v>
       </c>
@@ -10194,7 +10237,7 @@
       <c r="H18" s="10"/>
       <c r="I18" s="30"/>
     </row>
-    <row r="19" spans="2:9">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="30" t="s">
         <v>57</v>
       </c>
@@ -10216,7 +10259,7 @@
       <c r="H19" s="10"/>
       <c r="I19" s="30"/>
     </row>
-    <row r="20" spans="2:9">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="30" t="s">
         <v>57</v>
       </c>
@@ -10238,7 +10281,7 @@
       <c r="H20" s="10"/>
       <c r="I20" s="30"/>
     </row>
-    <row r="21" spans="2:9">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="30" t="s">
         <v>57</v>
       </c>
@@ -10260,7 +10303,7 @@
       <c r="H21" s="10"/>
       <c r="I21" s="30"/>
     </row>
-    <row r="22" spans="2:9" ht="29.1">
+    <row r="22" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B22" s="30" t="s">
         <v>57</v>
       </c>
@@ -10282,7 +10325,7 @@
       <c r="H22" s="10"/>
       <c r="I22" s="30"/>
     </row>
-    <row r="23" spans="2:9">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="30" t="s">
         <v>57</v>
       </c>
@@ -10302,7 +10345,7 @@
       <c r="H23" s="10"/>
       <c r="I23" s="30"/>
     </row>
-    <row r="24" spans="2:9">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" s="30" t="s">
         <v>57</v>
       </c>
@@ -10326,7 +10369,7 @@
       </c>
       <c r="I24" s="33"/>
     </row>
-    <row r="25" spans="2:9">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="30" t="s">
         <v>57</v>
       </c>
@@ -10350,7 +10393,7 @@
       </c>
       <c r="I25" s="33"/>
     </row>
-    <row r="26" spans="2:9">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" s="30" t="s">
         <v>57</v>
       </c>
@@ -10374,7 +10417,7 @@
       </c>
       <c r="I26" s="33"/>
     </row>
-    <row r="27" spans="2:9">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" s="30" t="s">
         <v>57</v>
       </c>
@@ -10398,7 +10441,7 @@
       </c>
       <c r="I27" s="33"/>
     </row>
-    <row r="28" spans="2:9">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" s="30" t="s">
         <v>57</v>
       </c>
@@ -10422,7 +10465,7 @@
       </c>
       <c r="I28" s="33"/>
     </row>
-    <row r="29" spans="2:9">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" s="30" t="s">
         <v>57</v>
       </c>
@@ -10446,7 +10489,7 @@
       </c>
       <c r="I29" s="33"/>
     </row>
-    <row r="30" spans="2:9">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" s="30" t="s">
         <v>57</v>
       </c>
@@ -10470,7 +10513,7 @@
       </c>
       <c r="I30" s="33"/>
     </row>
-    <row r="31" spans="2:9">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" s="30" t="s">
         <v>57</v>
       </c>
@@ -10494,7 +10537,7 @@
       </c>
       <c r="I31" s="33"/>
     </row>
-    <row r="32" spans="2:9">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" s="30" t="s">
         <v>57</v>
       </c>
@@ -10518,7 +10561,7 @@
       </c>
       <c r="I32" s="33"/>
     </row>
-    <row r="33" spans="2:9">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" s="30" t="s">
         <v>57</v>
       </c>
@@ -10540,7 +10583,7 @@
       <c r="H33" s="56"/>
       <c r="I33" s="30"/>
     </row>
-    <row r="34" spans="2:9" ht="15" thickBot="1">
+    <row r="34" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="35" t="s">
         <v>57</v>
       </c>
@@ -10564,7 +10607,7 @@
       </c>
       <c r="I34" s="13"/>
     </row>
-    <row r="35" spans="2:9" ht="15" thickBot="1">
+    <row r="35" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="265" t="s">
         <v>63</v>
       </c>
@@ -10588,7 +10631,7 @@
       </c>
       <c r="I35" s="13"/>
     </row>
-    <row r="36" spans="2:9">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" s="263" t="s">
         <v>64</v>
       </c>
@@ -10623,14 +10666,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AG41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="AE15" sqref="AE15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="6.42578125" customWidth="1"/>
     <col min="3" max="4" width="8" customWidth="1"/>
@@ -10646,8 +10689,8 @@
     <col min="15" max="15" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:33" ht="15" thickBot="1"/>
-    <row r="3" spans="1:33" ht="29.45" thickBot="1">
+    <row r="2" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:33" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="45" t="s">
         <v>65</v>
       </c>
@@ -10691,7 +10734,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:33">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" s="50" t="s">
         <v>47</v>
       </c>
@@ -10753,7 +10796,7 @@
       <c r="AF4" s="43"/>
       <c r="AG4" s="43"/>
     </row>
-    <row r="5" spans="1:33">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" s="51"/>
       <c r="B5" s="10">
         <v>2</v>
@@ -10813,7 +10856,7 @@
       <c r="AF5" s="44"/>
       <c r="AG5" s="44"/>
     </row>
-    <row r="6" spans="1:33">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="51"/>
       <c r="B6" s="10">
         <v>3</v>
@@ -10866,7 +10909,7 @@
       </c>
       <c r="AD6" s="5"/>
     </row>
-    <row r="7" spans="1:33">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" s="51"/>
       <c r="B7" s="10">
         <v>4</v>
@@ -10919,7 +10962,7 @@
       </c>
       <c r="AD7" s="5"/>
     </row>
-    <row r="8" spans="1:33">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" s="51"/>
       <c r="B8" s="10">
         <v>5</v>
@@ -10972,7 +11015,7 @@
       </c>
       <c r="AD8" s="5"/>
     </row>
-    <row r="9" spans="1:33">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" s="51"/>
       <c r="B9" s="10">
         <v>6</v>
@@ -11025,7 +11068,7 @@
       </c>
       <c r="AD9" s="5"/>
     </row>
-    <row r="10" spans="1:33">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" s="51"/>
       <c r="B10" s="10">
         <v>7</v>
@@ -11078,7 +11121,7 @@
       </c>
       <c r="AD10" s="5"/>
     </row>
-    <row r="11" spans="1:33">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" s="51"/>
       <c r="B11" s="10">
         <v>8</v>
@@ -11131,7 +11174,7 @@
       </c>
       <c r="AD11" s="5"/>
     </row>
-    <row r="12" spans="1:33">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" s="51"/>
       <c r="B12" s="10">
         <v>9</v>
@@ -11184,7 +11227,7 @@
       </c>
       <c r="AD12" s="5"/>
     </row>
-    <row r="13" spans="1:33" ht="15" thickBot="1">
+    <row r="13" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="52"/>
       <c r="B13" s="10">
         <v>10</v>
@@ -11237,7 +11280,7 @@
       </c>
       <c r="AD13" s="5"/>
     </row>
-    <row r="14" spans="1:33">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14" s="50" t="s">
         <v>53</v>
       </c>
@@ -11292,7 +11335,7 @@
       </c>
       <c r="AD14" s="5"/>
     </row>
-    <row r="15" spans="1:33">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" s="253"/>
       <c r="B15" s="10">
         <v>2</v>
@@ -11345,7 +11388,7 @@
       </c>
       <c r="AD15" s="5"/>
     </row>
-    <row r="16" spans="1:33">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A16" s="253"/>
       <c r="B16" s="10">
         <v>3</v>
@@ -11398,7 +11441,7 @@
       </c>
       <c r="AD16" s="5"/>
     </row>
-    <row r="17" spans="1:30">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A17" s="51"/>
       <c r="B17" s="10">
         <v>4</v>
@@ -11451,7 +11494,7 @@
       </c>
       <c r="AD17" s="5"/>
     </row>
-    <row r="18" spans="1:30">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A18" s="51"/>
       <c r="B18" s="10">
         <v>5</v>
@@ -11504,7 +11547,7 @@
       </c>
       <c r="AD18" s="5"/>
     </row>
-    <row r="19" spans="1:30">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A19" s="51"/>
       <c r="B19" s="38">
         <v>6</v>
@@ -11557,7 +11600,7 @@
       </c>
       <c r="AD19" s="5"/>
     </row>
-    <row r="20" spans="1:30" ht="15" thickBot="1">
+    <row r="20" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="52"/>
       <c r="B20" s="86">
         <v>7</v>
@@ -11610,7 +11653,7 @@
       </c>
       <c r="AD20" s="5"/>
     </row>
-    <row r="21" spans="1:30">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A21" s="53" t="s">
         <v>63</v>
       </c>
@@ -11665,7 +11708,7 @@
       </c>
       <c r="AD21" s="57"/>
     </row>
-    <row r="22" spans="1:30">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A22" s="43"/>
       <c r="B22" s="38">
         <v>2</v>
@@ -11718,7 +11761,7 @@
       </c>
       <c r="AD22" s="5"/>
     </row>
-    <row r="23" spans="1:30" ht="15" thickBot="1">
+    <row r="23" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="43"/>
       <c r="B23" s="84">
         <v>3</v>
@@ -11771,7 +11814,7 @@
       </c>
       <c r="AD23" s="5"/>
     </row>
-    <row r="24" spans="1:30" ht="15" thickBot="1">
+    <row r="24" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="54" t="s">
         <v>64</v>
       </c>
@@ -11826,7 +11869,7 @@
       </c>
       <c r="AD24" s="5"/>
     </row>
-    <row r="25" spans="1:30" ht="15" thickBot="1">
+    <row r="25" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="55"/>
       <c r="B25" s="5"/>
       <c r="C25" s="4"/>
@@ -11844,7 +11887,7 @@
       <c r="O25" s="5"/>
       <c r="AD25" s="5"/>
     </row>
-    <row r="26" spans="1:30">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A26" s="47" t="s">
         <v>53</v>
       </c>
@@ -11895,7 +11938,7 @@
       </c>
       <c r="AD26" s="5"/>
     </row>
-    <row r="27" spans="1:30">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A27" s="48"/>
       <c r="B27" s="38">
         <v>2</v>
@@ -11944,7 +11987,7 @@
       </c>
       <c r="AD27" s="5"/>
     </row>
-    <row r="28" spans="1:30">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A28" s="48"/>
       <c r="B28" s="38">
         <v>3</v>
@@ -11993,7 +12036,7 @@
       </c>
       <c r="AD28" s="5"/>
     </row>
-    <row r="29" spans="1:30">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A29" s="48"/>
       <c r="B29" s="38">
         <v>4</v>
@@ -12042,7 +12085,7 @@
       </c>
       <c r="AD29" s="5"/>
     </row>
-    <row r="30" spans="1:30">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A30" s="48"/>
       <c r="B30" s="39">
         <v>5</v>
@@ -12091,7 +12134,7 @@
       </c>
       <c r="AD30" s="5"/>
     </row>
-    <row r="31" spans="1:30">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A31" s="48"/>
       <c r="B31" s="38">
         <v>6</v>
@@ -12140,7 +12183,7 @@
       </c>
       <c r="AD31" s="5"/>
     </row>
-    <row r="32" spans="1:30">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A32" s="48"/>
       <c r="B32" s="38">
         <v>7</v>
@@ -12189,7 +12232,7 @@
       </c>
       <c r="AD32" s="5"/>
     </row>
-    <row r="33" spans="1:30" ht="15" thickBot="1">
+    <row r="33" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="49"/>
       <c r="B33" s="86">
         <v>8</v>
@@ -12238,7 +12281,7 @@
       </c>
       <c r="AD33" s="5"/>
     </row>
-    <row r="34" spans="1:30">
+    <row r="34" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A34" s="47" t="s">
         <v>47</v>
       </c>
@@ -12289,7 +12332,7 @@
       </c>
       <c r="AD34" s="5"/>
     </row>
-    <row r="35" spans="1:30">
+    <row r="35" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A35" s="48"/>
       <c r="B35" s="38">
         <v>2</v>
@@ -12338,7 +12381,7 @@
       </c>
       <c r="AD35" s="5"/>
     </row>
-    <row r="36" spans="1:30">
+    <row r="36" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A36" s="48"/>
       <c r="B36" s="38">
         <v>3</v>
@@ -12387,7 +12430,7 @@
       </c>
       <c r="AD36" s="5"/>
     </row>
-    <row r="37" spans="1:30">
+    <row r="37" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A37" s="48"/>
       <c r="B37" s="38">
         <v>4</v>
@@ -12436,7 +12479,7 @@
       </c>
       <c r="AD37" s="5"/>
     </row>
-    <row r="38" spans="1:30">
+    <row r="38" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A38" s="48"/>
       <c r="B38" s="38">
         <v>5</v>
@@ -12485,7 +12528,7 @@
       </c>
       <c r="AD38" s="5"/>
     </row>
-    <row r="39" spans="1:30">
+    <row r="39" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A39" s="48"/>
       <c r="B39" s="38">
         <v>6</v>
@@ -12534,7 +12577,7 @@
       </c>
       <c r="AD39" s="5"/>
     </row>
-    <row r="40" spans="1:30">
+    <row r="40" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A40" s="48"/>
       <c r="B40" s="38">
         <v>7</v>
@@ -12583,7 +12626,7 @@
       </c>
       <c r="AD40" s="5"/>
     </row>
-    <row r="41" spans="1:30" ht="15" thickBot="1">
+    <row r="41" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="49"/>
       <c r="B41" s="281">
         <v>8</v>
@@ -12624,4 +12667,146 @@
     <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:I13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5:G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="37" t="s">
+        <v>83</v>
+      </c>
+      <c r="E3" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="296" t="s">
+        <v>81</v>
+      </c>
+      <c r="G3" s="295" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4">
+        <v>158.6</v>
+      </c>
+      <c r="E4" s="30">
+        <v>158.6</v>
+      </c>
+      <c r="F4" s="5">
+        <v>1</v>
+      </c>
+      <c r="G4" s="41">
+        <f>0.002162/(E4/1000)-0.002756/SQRT(E4/1000)+0.003346</f>
+        <v>1.0057435036091411E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>25.271000000000001</v>
+      </c>
+      <c r="D5">
+        <v>100</v>
+      </c>
+      <c r="E5" s="298">
+        <f>(C5*D5+C6*D6)/(D5+D6)</f>
+        <v>25.192366013071894</v>
+      </c>
+      <c r="F5" s="297">
+        <v>1</v>
+      </c>
+      <c r="G5" s="299">
+        <f>0.002162/(E5/1000)-0.002756/SQRT(E5/1000)+0.003346</f>
+        <v>7.1801850267983594E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6">
+        <v>25.044</v>
+      </c>
+      <c r="D6">
+        <v>53</v>
+      </c>
+      <c r="E6" s="298"/>
+      <c r="F6" s="297"/>
+      <c r="G6" s="299"/>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7">
+        <v>28.486000000000001</v>
+      </c>
+      <c r="D7">
+        <v>17</v>
+      </c>
+      <c r="E7" s="298">
+        <f>(C7*D7+C8*D8)/(D7+D8)</f>
+        <v>28.47146153846154</v>
+      </c>
+      <c r="F7" s="297">
+        <v>0.2</v>
+      </c>
+      <c r="G7" s="299">
+        <f>0.002162/(E7/1000)-0.002756/SQRT(E7/1000)+0.003346</f>
+        <v>6.294837248963138E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8">
+        <v>28.443999999999999</v>
+      </c>
+      <c r="D8">
+        <v>9</v>
+      </c>
+      <c r="E8" s="298"/>
+      <c r="F8" s="297"/>
+      <c r="G8" s="299"/>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I13" s="294"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="G7:G8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>